<commit_message>
\#26: date format treatment updated.
</commit_message>
<xml_diff>
--- a/ecuacion-util-poi-sample/src/main/resources/sample.xlsx
+++ b/ecuacion-util-poi-sample/src/main/resources/sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yosuke.tanaka/Desktop/development/git/ecuacion-utils/ecuacion-util-poi-sample/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{312A9981-9396-0B4C-B66E-3A875BC67587}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7ED6F70-A570-0D41-878C-60ECF204C898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{A877D16A-EB0C-794F-9DC4-B2BFC1BC3DCE}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16660" xr2:uid="{A877D16A-EB0C-794F-9DC4-B2BFC1BC3DCE}"/>
   </bookViews>
   <sheets>
     <sheet name="Member" sheetId="1" r:id="rId1"/>
@@ -81,6 +81,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="180" formatCode="m/d/yy;@"/>
+  </numFmts>
   <fonts count="4">
     <font>
       <sz val="12"/>
@@ -160,7 +163,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -174,6 +177,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -513,7 +519,7 @@
   <dimension ref="B1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -553,7 +559,7 @@
       <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="5">
         <v>28126</v>
       </c>
       <c r="E4" s="2">

</xml_diff>

<commit_message>
\#30: feature to read time format to string added.
Besides, unneeded comments deleted.
</commit_message>
<xml_diff>
--- a/ecuacion-util-poi-sample/src/main/resources/sample.xlsx
+++ b/ecuacion-util-poi-sample/src/main/resources/sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yosuke.tanaka/Desktop/development/git/ecuacion-utils/ecuacion-util-poi-sample/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7ED6F70-A570-0D41-878C-60ECF204C898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEBDADA5-AC92-1C4A-A186-347AEC7832FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16660" xr2:uid="{A877D16A-EB0C-794F-9DC4-B2BFC1BC3DCE}"/>
   </bookViews>
@@ -82,7 +82,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="180" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="176" formatCode="m/d/yy;@"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -179,7 +179,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -519,14 +519,14 @@
   <dimension ref="B1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
   <cols>
     <col min="1" max="1" width="1.7109375" customWidth="1"/>
     <col min="2" max="2" width="5.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6" customWidth="1"/>
   </cols>
   <sheetData>
@@ -560,7 +560,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="5">
-        <v>28126</v>
+        <v>28126.058159722223</v>
       </c>
       <c r="E4" s="2">
         <v>47</v>

</xml_diff>

<commit_message>
\#44: reader and writer now can starts and ends with workbook.
</commit_message>
<xml_diff>
--- a/ecuacion-util-poi-sample/src/main/resources/sample.xlsx
+++ b/ecuacion-util-poi-sample/src/main/resources/sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yosuke.tanaka/Desktop/development/git/ecuacion-utils/ecuacion-util-poi-sample/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEBDADA5-AC92-1C4A-A186-347AEC7832FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCECAB25-94AB-0E49-B6C7-CA18BE77BA4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16660" xr2:uid="{A877D16A-EB0C-794F-9DC4-B2BFC1BC3DCE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1"/>
@@ -74,6 +74,10 @@
   </si>
   <si>
     <t>Member list</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>(in sample.xlsx)</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -519,20 +523,21 @@
   <dimension ref="B1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
   <cols>
     <col min="1" max="1" width="1.7109375" customWidth="1"/>
-    <col min="2" max="2" width="5.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6" customWidth="1"/>
+    <col min="2" max="6" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6">
       <c r="B1" s="4" t="s">
         <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="2:6">

</xml_diff>